<commit_message>
Labs 1 & 6 tex outline
</commit_message>
<xml_diff>
--- a/Lab5-P1,6-PlancksConstant&BlackbodyRadiation/P6-BlackbodyRadiation/Data2/3volt_processed.xlsx
+++ b/Lab5-P1,6-PlancksConstant&BlackbodyRadiation/P6-BlackbodyRadiation/Data2/3volt_processed.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,31 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarah\Documents\GitHub\SeniorLab\Lab5-P1,6-PlancksConstant&amp;BlackbodyRadiation\P6-BlackbodyRadiation\Data2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{605D9137-DBD3-47C5-BDA0-612AA7D3CF81}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497DD475-CC53-4D02-8F0C-AFF2CF6EE0BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3volt_processed" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
-  <si>
-    <t>Set</t>
-  </si>
-  <si>
-    <t>Run #1</t>
-  </si>
-  <si>
-    <t>Angle deg (units)</t>
-  </si>
-  <si>
-    <t>Time (s)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Relative Intensity (%)</t>
   </si>
@@ -40,28 +36,46 @@
     <t>Theo lambda max</t>
   </si>
   <si>
-    <t>Bulb Voltage [V]</t>
-  </si>
-  <si>
-    <t>Bulb Current [I]</t>
-  </si>
-  <si>
     <t>Calculated Bulb Resistance [Ohm]</t>
   </si>
   <si>
-    <t>Temperature [K]</t>
+    <t>Calculated index</t>
   </si>
   <si>
-    <t>Calc. index</t>
+    <t>Measured Bulb Voltage [V]</t>
   </si>
   <si>
-    <t>Calc. lambda</t>
+    <t>Measured Bulb Current [I]</t>
+  </si>
+  <si>
+    <t>Calculated Temperature [K]</t>
+  </si>
+  <si>
+    <t>Calculated Bulb Resistivity</t>
+  </si>
+  <si>
+    <t>Raw reading</t>
+  </si>
+  <si>
+    <t>Angle [deg]</t>
+  </si>
+  <si>
+    <t>Calc lambda [nm]</t>
+  </si>
+  <si>
+    <t>lambda [um]</t>
+  </si>
+  <si>
+    <t>Experimental Determination of Peak Wavelength</t>
+  </si>
+  <si>
+    <t>Theoretical Determination of Peak Wavelength</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -539,9 +553,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -625,7 +640,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'3volt_processed'!$C$2</c:f>
+              <c:f>'3volt_processed'!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -658,7 +673,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'3volt_processed'!$E$3:$E$17</c:f>
+              <c:f>'3volt_processed'!$E$4:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -678,22 +693,22 @@
                   <c:v>391.29718117397016</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>408.03851051198865</c:v>
+                  <c:v>408.03851051198927</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>427.88479997419387</c:v>
+                  <c:v>427.88479997419324</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>451.81656713969318</c:v>
+                  <c:v>451.81656713969392</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>481.31649332822707</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>518.75591152431173</c:v>
+                  <c:v>518.75591152431275</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>568.22030490570216</c:v>
+                  <c:v>568.22030490570512</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>637.51804564298061</c:v>
@@ -712,7 +727,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'3volt_processed'!$C$3:$C$17</c:f>
+              <c:f>'3volt_processed'!$C$4:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1052,37 +1067,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1687,16 +1671,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>471487</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>74612</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>515937</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>166687</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>7937</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>530225</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2020,384 +2004,480 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="7.6796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.04296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A3">
-        <v>110</v>
-      </c>
-      <c r="B3">
-        <v>665.9</v>
-      </c>
-      <c r="C3">
-        <v>-0.74</v>
-      </c>
-      <c r="D3">
-        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(A3)) + 0.5 )^2 + 0.75)</f>
-        <v>1.8062188508627124</v>
-      </c>
-      <c r="E3">
-        <f>SQRT(13900 / (D3-1.689) )</f>
-        <v>344.35680552035296</v>
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4">
-        <v>682.35</v>
+        <f>180-A4</f>
+        <v>70</v>
       </c>
       <c r="C4">
-        <v>-0.59</v>
+        <v>-0.74</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D19" si="0">SQRT(( (2/SQRT(3))*SIN(RADIANS(A4)) + 0.5 )^2 + 0.75)</f>
-        <v>1.8000284362795256</v>
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B4)) + 0.5 )^2 + 0.75)</f>
+        <v>1.8062188508627124</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E19" si="1">SQRT(13900 / (D4-1.689) )</f>
-        <v>353.82644461019186</v>
+        <f>SQRT(13900 / (D4-1.689) )</f>
+        <v>344.35680552035296</v>
+      </c>
+      <c r="F4">
+        <f>E4/1000</f>
+        <v>0.34435680552035297</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B5">
-        <v>705</v>
+        <f t="shared" ref="B5:B19" si="0">180-A5</f>
+        <v>69</v>
       </c>
       <c r="C5">
-        <v>-0.72</v>
+        <v>-0.59</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>1.7935568654503042</v>
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B5)) + 0.5 )^2 + 0.75)</f>
+        <v>1.8000284362795256</v>
       </c>
       <c r="E5">
-        <f t="shared" si="1"/>
-        <v>364.61213832370197</v>
+        <f t="shared" ref="E5:E20" si="1">SQRT(13900 / (D5-1.689) )</f>
+        <v>353.82644461019186</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F18" si="2">E5/1000</f>
+        <v>0.35382644461019186</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B6">
-        <v>721</v>
+        <f t="shared" si="0"/>
+        <v>68</v>
       </c>
       <c r="C6">
-        <v>-0.45</v>
+        <v>-0.72</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>1.7868071235684373</v>
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B6)) + 0.5 )^2 + 0.75)</f>
+        <v>1.7935568654503042</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>376.98333898391292</v>
+        <v>364.61213832370197</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>0.36461213832370198</v>
+      </c>
+      <c r="H6">
+        <v>0.38800000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A7">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7">
-        <v>749.1</v>
+        <f t="shared" si="0"/>
+        <v>67</v>
       </c>
       <c r="C7">
-        <v>-0.4</v>
+        <v>-0.45</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>1.7797823376318811</v>
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B7)) + 0.5 )^2 + 0.75)</f>
+        <v>1.7868071235684373</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>391.29718117397016</v>
+        <v>376.98333898391292</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>0.3769833389839129</v>
       </c>
       <c r="H7" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8">
-        <v>768.7</v>
+        <f t="shared" si="0"/>
+        <v>66</v>
       </c>
       <c r="C8">
-        <v>-0.57999999999999996</v>
+        <v>-0.4</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1.7724857769301154</v>
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B8)) + 0.5 )^2 + 0.75)</f>
+        <v>1.7797823376318811</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>408.03851051198865</v>
+        <v>391.29718117397016</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>0.39129718117397017</v>
+      </c>
+      <c r="H8">
+        <f>H4/H6</f>
+        <v>7.731958762886598</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A9">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B9">
-        <v>801.95</v>
+        <f t="shared" si="0"/>
+        <v>65</v>
       </c>
       <c r="C9">
-        <v>-0.6</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>1.7649208535712926</v>
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B9)) + 0.5 )^2 + 0.75)</f>
+        <v>1.7724857769301152</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>427.88479997419387</v>
+        <v>408.03851051198927</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>0.40803851051198925</v>
       </c>
       <c r="H9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A10">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B10">
-        <v>834.2</v>
+        <f t="shared" si="0"/>
+        <v>64</v>
       </c>
       <c r="C10">
-        <v>-0.62</v>
+        <v>-0.6</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>1.7570911230519748</v>
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B10)) + 0.5 )^2 + 0.75)</f>
+        <v>1.7649208535712928</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>451.81656713969318</v>
-      </c>
-      <c r="H10" t="e">
-        <f>0.002898/H8</f>
-        <v>#DIV/0!</v>
+        <v>427.88479997419324</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>0.42788479997419326</v>
+      </c>
+      <c r="H10">
+        <f>5.65*((H8-0.2)/0.93)</f>
+        <v>45.758674204633635</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A11">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B11">
-        <v>850.15</v>
+        <f t="shared" si="0"/>
+        <v>63</v>
       </c>
       <c r="C11">
-        <v>-0.6</v>
+        <v>-0.62</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>1.7490002848719128</v>
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B11)) + 0.5 )^2 + 0.75)</f>
+        <v>1.7570911230519746</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>481.31649332822707</v>
+        <v>451.81656713969392</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>0.45181656713969393</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A12">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B12">
-        <v>894.35</v>
+        <f t="shared" si="0"/>
+        <v>62</v>
       </c>
       <c r="C12">
-        <v>-0.51</v>
+        <v>-0.6</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>1.7406521831964117</v>
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B12)) + 0.5 )^2 + 0.75)</f>
+        <v>1.7490002848719128</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>518.75591152431173</v>
+        <v>481.31649332822707</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>0.48131649332822707</v>
+      </c>
+      <c r="H12">
+        <f>103 + (38.1*H10) - (0.095*H10*H10) + ((2.48*10^(-4))*(H10^3))</f>
+        <v>1671.2505395164458</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A13">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B13">
-        <v>909.05</v>
+        <f t="shared" si="0"/>
+        <v>61</v>
       </c>
       <c r="C13">
-        <v>-0.53</v>
+        <v>-0.51</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>1.7320508075688776</v>
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B13)) + 0.5 )^2 + 0.75)</f>
+        <v>1.7406521831964115</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>568.22030490570216</v>
+        <v>518.75591152431275</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>0.51875591152431277</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A14">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B14">
-        <v>940.25</v>
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="C14">
-        <v>-0.6</v>
+        <v>-0.53</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>1.7232002936762014</v>
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B14)) + 0.5 )^2 + 0.75)</f>
+        <v>1.7320508075688772</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>637.51804564298061</v>
+        <v>568.22030490570512</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>0.56822030490570508</v>
+      </c>
+      <c r="H14">
+        <f>0.002898/H12</f>
+        <v>1.7340308538290721E-6</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A15">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B15">
-        <v>1002.7</v>
+        <f t="shared" si="0"/>
+        <v>59</v>
       </c>
       <c r="C15">
-        <v>-0.52</v>
+        <v>-0.6</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>1.71410492416967</v>
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B15)) + 0.5 )^2 + 0.75)</f>
+        <v>1.7232002936762014</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>744.09424081455097</v>
+        <v>637.51804564298061</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>0.63751804564298065</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A16">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B16">
-        <v>1018.5</v>
+        <f t="shared" si="0"/>
+        <v>58</v>
       </c>
       <c r="C16">
-        <v>0.03</v>
+        <v>-0.52</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>1.7047691295441194</v>
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B16)) + 0.5 )^2 + 0.75)</f>
+        <v>1.71410492416967</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>938.86584394116119</v>
+        <v>744.09424081455097</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>0.744094240814551</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A17">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B17">
-        <v>1052.2</v>
+        <f t="shared" si="0"/>
+        <v>57</v>
       </c>
       <c r="C17">
-        <v>-0.15</v>
+        <v>0.03</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>1.6951974890780552</v>
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B17)) + 0.5 )^2 + 0.75)</f>
+        <v>1.7047691295441194</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
+        <v>938.86584394116119</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>0.93886584394116124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A18">
+        <v>124</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="C18">
+        <v>-0.15</v>
+      </c>
+      <c r="D18">
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B18)) + 0.5 )^2 + 0.75)</f>
+        <v>1.6951974890780552</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
         <v>1497.6127027294388</v>
       </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>1.4976127027294388</v>
+      </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A18" s="1">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A19" s="1">
         <v>125</v>
       </c>
-      <c r="B18" s="1">
-        <v>1077.25</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="B19" s="1">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="C19" s="1">
         <v>-0.38</v>
       </c>
-      <c r="D18" s="1">
-        <f t="shared" si="0"/>
-        <v>1.6853947318374436</v>
-      </c>
-      <c r="E18" s="1" t="e">
+      <c r="D19" s="1">
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B19)) + 0.5 )^2 + 0.75)</f>
+        <v>1.685394731837444</v>
+      </c>
+      <c r="E19" s="1" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1">
-        <v>195.15</v>
-      </c>
-      <c r="C19" s="1">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1">
         <v>-1.35</v>
       </c>
-      <c r="D19" s="1">
-        <f t="shared" si="0"/>
+      <c r="D20" s="1">
+        <f>SQRT(( (2/SQRT(3))*SIN(RADIANS(B20)) + 0.5 )^2 + 0.75)</f>
         <v>1</v>
       </c>
-      <c r="E19" s="1" t="e">
+      <c r="E20" s="1" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>

</xml_diff>